<commit_message>
+ custimized item_category. + custimized item_type2category. + dat/all_item_export for andromoney export format + fix typo type: Electicity, Transpotation, Entertainmant,
</commit_message>
<xml_diff>
--- a/TRUNK/dat/excel/My_account_example.xlsx
+++ b/TRUNK/dat/excel/My_account_example.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\tonychenglx\pwa\homeproj\GitHub\myaccount2p0\TRUNK\dat\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B011EF-D7AB-427D-8355-1944928CB822}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94048EA-5C05-4C6E-8C86-E15594BC8248}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,9 +62,6 @@
     <t>Dinner</t>
   </si>
   <si>
-    <t>Transpotation</t>
-  </si>
-  <si>
     <t>Supplyment</t>
   </si>
   <si>
@@ -81,12 +78,6 @@
   </si>
   <si>
     <t>Rental</t>
-  </si>
-  <si>
-    <t>Electicity</t>
-  </si>
-  <si>
-    <t>Entertainmant</t>
   </si>
   <si>
     <t>Bonus</t>
@@ -238,6 +229,18 @@
   </si>
   <si>
     <t>Borrow</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entertainment</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Transportation</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Electricity</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -844,7 +847,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -856,7 +859,7 @@
   <sheetData>
     <row r="1" spans="1:1024">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AGL1"/>
       <c r="AGM1"/>
@@ -4243,7 +4246,7 @@
     </row>
     <row r="4" spans="1:1024">
       <c r="A4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -7329,7 +7332,7 @@
     </row>
     <row r="7" spans="1:1024">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -8357,7 +8360,7 @@
     </row>
     <row r="8" spans="1:1024">
       <c r="A8" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -9385,7 +9388,7 @@
     </row>
     <row r="9" spans="1:1024">
       <c r="A9" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -10413,7 +10416,7 @@
     </row>
     <row r="10" spans="1:1024">
       <c r="A10" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -11441,7 +11444,7 @@
     </row>
     <row r="11" spans="1:1024">
       <c r="A11" s="4" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -12469,7 +12472,7 @@
     </row>
     <row r="12" spans="1:1024">
       <c r="A12" s="10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -13497,7 +13500,7 @@
     </row>
     <row r="13" spans="1:1024">
       <c r="A13" s="10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -14525,7 +14528,7 @@
     </row>
     <row r="14" spans="1:1024">
       <c r="A14" s="10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -15553,7 +15556,7 @@
     </row>
     <row r="15" spans="1:1024">
       <c r="A15" s="10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -16581,7 +16584,7 @@
     </row>
     <row r="16" spans="1:1024">
       <c r="A16" s="10" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
@@ -17609,7 +17612,7 @@
     </row>
     <row r="17" spans="1:1024">
       <c r="A17" s="10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
@@ -18637,7 +18640,7 @@
     </row>
     <row r="18" spans="1:1024">
       <c r="A18" s="10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
@@ -19665,7 +19668,7 @@
     </row>
     <row r="19" spans="1:1024" s="15" customFormat="1">
       <c r="A19" s="11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -20538,7 +20541,7 @@
     </row>
     <row r="20" spans="1:1024" s="15" customFormat="1">
       <c r="A20" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
@@ -21411,7 +21414,7 @@
     </row>
     <row r="21" spans="1:1024" s="15" customFormat="1">
       <c r="A21" s="11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -22284,7 +22287,7 @@
     </row>
     <row r="22" spans="1:1024">
       <c r="A22" s="12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
@@ -23312,7 +23315,7 @@
     </row>
     <row r="23" spans="1:1024">
       <c r="A23" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
@@ -24340,7 +24343,7 @@
     </row>
     <row r="24" spans="1:1024">
       <c r="A24" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
@@ -25368,7 +25371,7 @@
     </row>
     <row r="25" spans="1:1024">
       <c r="A25" s="12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
@@ -26396,7 +26399,7 @@
     </row>
     <row r="26" spans="1:1024">
       <c r="A26" s="12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
@@ -27424,7 +27427,7 @@
     </row>
     <row r="27" spans="1:1024">
       <c r="A27" s="12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
@@ -28452,7 +28455,7 @@
     </row>
     <row r="28" spans="1:1024">
       <c r="A28" s="12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
@@ -29480,7 +29483,7 @@
     </row>
     <row r="29" spans="1:1024">
       <c r="A29" s="12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -30508,7 +30511,7 @@
     </row>
     <row r="30" spans="1:1024">
       <c r="A30" s="12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
@@ -31536,7 +31539,7 @@
     </row>
     <row r="31" spans="1:1024">
       <c r="A31" s="12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
@@ -32564,7 +32567,7 @@
     </row>
     <row r="32" spans="1:1024" s="17" customFormat="1">
       <c r="A32" s="16" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -33437,7 +33440,7 @@
     </row>
     <row r="33" spans="1:1024">
       <c r="A33" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -34465,7 +34468,7 @@
     </row>
     <row r="34" spans="1:1024">
       <c r="A34" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -35493,7 +35496,7 @@
     </row>
     <row r="35" spans="1:1024">
       <c r="A35" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -36521,7 +36524,7 @@
     </row>
     <row r="36" spans="1:1024" s="21" customFormat="1">
       <c r="A36" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B36" s="19"/>
       <c r="C36" s="20"/>
@@ -37394,7 +37397,7 @@
     </row>
     <row r="37" spans="1:1024" s="21" customFormat="1">
       <c r="A37" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B37" s="19"/>
       <c r="C37" s="20"/>
@@ -38267,7 +38270,7 @@
     </row>
     <row r="38" spans="1:1024" s="21" customFormat="1">
       <c r="A38" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B38" s="19"/>
       <c r="C38" s="20"/>
@@ -39140,7 +39143,7 @@
     </row>
     <row r="39" spans="1:1024" s="21" customFormat="1">
       <c r="A39" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B39" s="19"/>
       <c r="C39" s="20"/>
@@ -40013,7 +40016,7 @@
     </row>
     <row r="40" spans="1:1024" s="21" customFormat="1">
       <c r="A40" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B40" s="19"/>
       <c r="C40" s="20"/>
@@ -40886,7 +40889,7 @@
     </row>
     <row r="41" spans="1:1024" s="21" customFormat="1">
       <c r="A41" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B41" s="19"/>
       <c r="C41" s="20"/>
@@ -41759,7 +41762,7 @@
     </row>
     <row r="42" spans="1:1024" s="21" customFormat="1">
       <c r="A42" s="9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B42" s="19"/>
       <c r="C42" s="20"/>
@@ -42632,7 +42635,7 @@
     </row>
     <row r="43" spans="1:1024" s="21" customFormat="1">
       <c r="A43" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B43" s="19"/>
       <c r="C43" s="20"/>
@@ -43505,7 +43508,7 @@
     </row>
     <row r="44" spans="1:1024" s="21" customFormat="1">
       <c r="A44" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B44" s="19"/>
       <c r="C44" s="20"/>
@@ -44378,7 +44381,7 @@
     </row>
     <row r="45" spans="1:1024" s="21" customFormat="1">
       <c r="A45" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B45" s="19"/>
       <c r="C45" s="20"/>
@@ -45251,7 +45254,7 @@
     </row>
     <row r="46" spans="1:1024" s="21" customFormat="1">
       <c r="A46" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B46" s="19"/>
       <c r="C46" s="20"/>
@@ -46124,7 +46127,7 @@
     </row>
     <row r="47" spans="1:1024" s="21" customFormat="1">
       <c r="A47" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B47" s="19"/>
       <c r="C47" s="20"/>
@@ -46997,7 +47000,7 @@
     </row>
     <row r="48" spans="1:1024" s="21" customFormat="1">
       <c r="A48" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B48" s="19"/>
       <c r="C48" s="20"/>
@@ -47870,7 +47873,7 @@
     </row>
     <row r="49" spans="1:869" s="21" customFormat="1">
       <c r="A49" s="9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B49" s="19"/>
       <c r="C49" s="20"/>
@@ -48743,7 +48746,7 @@
     </row>
     <row r="50" spans="1:869" s="18" customFormat="1" ht="16.5" customHeight="1">
       <c r="A50" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
@@ -49616,7 +49619,7 @@
     </row>
     <row r="51" spans="1:869">
       <c r="A51" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>